<commit_message>
Publish v1 of Jibres Investment pack
</commit_message>
<xml_diff>
--- a/business/financial/Jibres-Financial-Projection-v1.xlsx
+++ b/business/financial/Jibres-Financial-Projection-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\projects\talambar_cdn\business\financial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDF5B8FD-26C5-4522-AAE0-074B4C3A365A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C76743-9823-4974-BD81-339C07EAFD95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="865" activeTab="11" xr2:uid="{6B758C63-8066-4742-BFF0-F2DCF7A6BA0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="865" activeTab="10" xr2:uid="{6B758C63-8066-4742-BFF0-F2DCF7A6BA0C}"/>
   </bookViews>
   <sheets>
     <sheet name="خلاصه هزینه‌ها" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <definedName name="v_seriF">'مراحل سرمایه‌گذاری'!$M$8</definedName>
     <definedName name="v_totalFund">'خلاصه و ارزیابی'!$C$16</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <webPublishing allowPng="1" targetScreenSize="1800x1440" codePage="65001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -13807,8 +13807,8 @@
   </sheetPr>
   <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="17.25" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -14272,27 +14272,27 @@
       </c>
       <c r="D13" s="59">
         <f t="shared" ref="D13:I13" si="6">D12/v_totalFund</f>
-        <v>-0.27539960526315788</v>
+        <v>-0.20930370000000001</v>
       </c>
       <c r="E13" s="59">
         <f t="shared" si="6"/>
-        <v>-0.55940092105263162</v>
+        <v>-0.42514469999999999</v>
       </c>
       <c r="F13" s="59">
         <f t="shared" si="6"/>
-        <v>-0.23638105263157894</v>
+        <v>-0.17964959999999999</v>
       </c>
       <c r="G13" s="59">
         <f t="shared" si="6"/>
-        <v>2.4417762039473678</v>
+        <v>1.8557499149999996</v>
       </c>
       <c r="H13" s="59">
         <f t="shared" si="6"/>
-        <v>13.15003936480263</v>
+        <v>9.994029917249998</v>
       </c>
       <c r="I13" s="59">
         <f t="shared" si="6"/>
-        <v>49.998561560970387</v>
+        <v>37.998906786337493</v>
       </c>
       <c r="J13" s="59"/>
     </row>
@@ -14318,8 +14318,7 @@
         <v>190</v>
       </c>
       <c r="C16" s="61">
-        <f>ROUND(SUM(tbl_sumary[[1400]:[1401]]),-7 )</f>
-        <v>15200000000</v>
+        <v>20000000000</v>
       </c>
       <c r="D16" s="61"/>
       <c r="E16" s="61"/>
@@ -14752,7 +14751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AB18F9-F9BE-4D2E-8E8A-5E7D56BD756A}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>